<commit_message>
TC User reg. update
</commit_message>
<xml_diff>
--- a/Test Cases User Registration.xlsx
+++ b/Test Cases User Registration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tnikolova\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgyurov\Desktop\PetStoreTestingTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,8 +18,34 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Martin Gyurov</author>
+  </authors>
+  <commentList>
+    <comment ref="D11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Martin Gyurov:
+Too mu</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="134">
   <si>
     <t>TC Title</t>
   </si>
@@ -1138,12 +1164,63 @@
   <si>
     <t>The field for the birthday date input matches the date chosen from the calendar</t>
   </si>
+  <si>
+    <t>1. Leave all fields empty 
+2.Click submit button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Leave all fields empty
+2.Check 1-3 subscriptions
+3.Click submit button </t>
+  </si>
+  <si>
+    <t>1.Leave Address field empty
+2.Fill all other required fields with Valid data
+3.Check on 0-3 subscriptions (optional)
+4.Click submit button</t>
+  </si>
+  <si>
+    <t>1.Leave Birthday field empty
+2.Fill all other required fields with Valid data
+3.Check on 0-3 subscriptions (optional)
+4.Click submit button</t>
+  </si>
+  <si>
+    <t>1.Leave Confirm password field empty
+2.Fill all other required fields with Valid data
+3.Check on 0-3 subscriptions (optional)
+4.Click submit button</t>
+  </si>
+  <si>
+    <t>1.Leave Password field empty
+2.Fill all other required fields with Valid data
+3.Check on 0-3 subscriptions (optional)
+4.Click submit button</t>
+  </si>
+  <si>
+    <t>1.Leave Username field empty
+2.Fill all other required fields with Valid data
+3.Check on 0-3 subscriptions (optional)
+4.Click submit button</t>
+  </si>
+  <si>
+    <t>1.In Username field type only 1 character
+2.Fill all other required fields with Valid data
+3.Check on 0-3 subscriptions (optional)
+4.Click submit button</t>
+  </si>
+  <si>
+    <t>could be written as 1 TC</t>
+  </si>
+  <si>
+    <t>TC can faild both at step 2 and step 3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1161,21 +1238,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1215,8 +1277,32 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1235,8 +1321,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1257,12 +1349,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1273,71 +1380,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1643,696 +1761,744 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="65.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="65" customWidth="1"/>
+    <col min="6" max="6" width="65" style="15" customWidth="1"/>
+    <col min="7" max="7" width="0.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="14" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="22" t="s">
         <v>4</v>
       </c>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:9" ht="156" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="22" t="s">
         <v>4</v>
       </c>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="20" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="21" t="s">
         <v>36</v>
       </c>
+      <c r="G9" s="16" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="20">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="G10" s="11" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="20">
         <v>7</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="23" t="s">
         <v>44</v>
       </c>
+      <c r="G11" s="11" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="20">
         <v>8</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="G12" s="11" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="20">
         <v>9</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="23" t="s">
         <v>40</v>
       </c>
+      <c r="G13" s="11" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="20">
         <v>10</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="23" t="s">
         <v>46</v>
       </c>
+      <c r="G14" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="20">
         <v>11</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="23" t="s">
         <v>45</v>
       </c>
+      <c r="G15" s="11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" s="11" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23">
+      <c r="C16" s="26"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" s="5" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25">
         <v>12</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" s="11" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23">
+      <c r="F17" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
         <v>13</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" s="11" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23">
+      <c r="F18" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
         <v>14</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23">
+      <c r="A20" s="25">
         <v>15</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23">
+      <c r="A21" s="25">
         <v>16</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23">
+      <c r="A22" s="25">
         <v>17</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23">
+      <c r="A23" s="25">
         <v>18</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23">
+      <c r="A24" s="25">
         <v>19</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="4"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26" spans="1:6" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23">
+      <c r="A26" s="25">
         <v>20</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="F26" s="29" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23">
+      <c r="A27" s="25">
         <v>21</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="23">
+      <c r="A28" s="25">
         <v>22</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="F28" s="29"/>
     </row>
     <row r="29" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23">
+      <c r="A29" s="25">
         <v>23</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="F29" s="29"/>
     </row>
     <row r="30" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23">
+      <c r="A30" s="25">
         <v>24</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="F30" s="29"/>
     </row>
     <row r="31" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23">
+      <c r="A31" s="25">
         <v>25</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="F31" s="29"/>
     </row>
     <row r="32" spans="1:6" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23">
+      <c r="A32" s="25">
         <v>26</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23">
+      <c r="A33" s="25">
         <v>27</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:6" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="23">
+      <c r="A34" s="25">
         <v>28</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="23">
+      <c r="A35" s="25">
         <v>29</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="4"/>
-      <c r="F36" s="5"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="23">
+      <c r="A37" s="25">
         <v>30</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="5"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="4"/>
-      <c r="F38" s="5"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="23">
+      <c r="A39" s="25">
         <v>31</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F39" s="5"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="5"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+      <c r="A41" s="20">
         <v>32</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+      <c r="A42" s="20">
         <v>33</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43" s="20">
         <v>34</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="23" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2356,5 +2522,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TC Search page update
</commit_message>
<xml_diff>
--- a/Test Cases User Registration.xlsx
+++ b/Test Cases User Registration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzhingova\Desktop\PetStoreTestingTask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgyurov\Desktop\PetStoreTestingTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -488,6 +488,10 @@
     <t>TC can faild both at step 2 and step 3</t>
   </si>
   <si>
+    <t xml:space="preserve">
+1. Click submit button</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1. Username field is empty
 2. Password field is empty
@@ -499,7 +503,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -509,7 +513,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -521,7 +525,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -531,7 +535,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -553,7 +557,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -563,7 +567,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -585,7 +589,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -595,7 +599,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -617,7 +621,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -627,7 +631,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -649,7 +653,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -659,7 +663,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -673,7 +677,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -683,7 +687,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -701,7 +705,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -711,7 +715,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -729,7 +733,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -739,7 +743,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -757,7 +761,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -767,7 +771,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -785,7 +789,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -795,7 +799,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -813,7 +817,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -824,7 +828,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -842,7 +846,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -852,7 +856,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -870,7 +874,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -880,7 +884,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -902,7 +906,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -912,7 +916,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -933,7 +937,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -943,7 +947,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -964,7 +968,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -974,7 +978,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -995,7 +999,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -1005,7 +1009,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1026,7 +1030,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -1036,7 +1040,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1057,7 +1061,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -1067,7 +1071,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1088,7 +1092,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -1098,7 +1102,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1119,7 +1123,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -1129,7 +1133,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1150,7 +1154,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -1160,7 +1164,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1181,7 +1185,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -1191,7 +1195,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1204,23 +1208,14 @@
 7.  Mark none/ one/ two/ three options from the subscriptions menu
 8.Click submit button</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. Click submit button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -1267,14 +1262,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1282,34 +1269,14 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1381,112 +1348,87 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1795,796 +1737,750 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="65" style="15" customWidth="1"/>
-    <col min="7" max="7" width="0.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" style="27" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="65" style="8" customWidth="1"/>
+    <col min="7" max="7" width="0.140625" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="14.42578125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:9" s="15" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="156" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="14"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" s="18" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:9" s="5" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" s="20" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="19">
         <v>5</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16">
+        <v>9</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="16">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
+      <c r="B16" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" s="20" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <v>12</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="20" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19">
+        <v>13</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="20" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="19">
+        <v>14</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="19">
+        <v>15</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19">
+        <v>16</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="19">
+        <v>17</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="19">
+        <v>18</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="19">
+        <v>19</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="19">
+        <v>20</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="19">
+        <v>21</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="19">
+        <v>22</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="25"/>
+    </row>
+    <row r="29" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="19">
+        <v>23</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="25"/>
+    </row>
+    <row r="30" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="19">
+        <v>24</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="25"/>
+    </row>
+    <row r="31" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="19">
+        <v>25</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="25"/>
+    </row>
+    <row r="32" spans="1:6" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="19">
+        <v>26</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="19">
+        <v>27</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:6" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="19">
+        <v>28</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="19">
+        <v>29</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="32">
-        <v>6</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="32">
-        <v>7</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32">
-        <v>8</v>
-      </c>
-      <c r="B12" s="29" t="s">
+      <c r="E35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="25"/>
+    </row>
+    <row r="36" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="19">
         <v>30</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32">
+      <c r="B37" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="19">
+        <v>31</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="16">
+        <v>32</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="32">
+      <c r="E41" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="16">
+        <v>33</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32">
+      <c r="E42" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="16">
+        <v>34</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32"/>
-      <c r="B16" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28">
-        <v>12</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="30"/>
-    </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
+      <c r="E43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
-        <v>14</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="30"/>
-    </row>
-    <row r="20" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28">
-        <v>15</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="27"/>
-    </row>
-    <row r="21" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="28">
-        <v>16</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
-    </row>
-    <row r="22" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="28">
-        <v>17</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28">
-        <v>18</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="28">
-        <v>19</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
-    </row>
-    <row r="25" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-    </row>
-    <row r="26" spans="1:7" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28">
-        <v>20</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="27"/>
-    </row>
-    <row r="27" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28">
-        <v>21</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="27"/>
-    </row>
-    <row r="28" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="28">
-        <v>22</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="27"/>
-    </row>
-    <row r="29" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="28">
-        <v>23</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="27"/>
-    </row>
-    <row r="30" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="28">
-        <v>24</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="27"/>
-    </row>
-    <row r="31" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="28">
-        <v>25</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="27"/>
-    </row>
-    <row r="32" spans="1:7" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="28">
-        <v>26</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="27"/>
-    </row>
-    <row r="33" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="28">
-        <v>27</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="27"/>
-    </row>
-    <row r="34" spans="1:7" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="28">
-        <v>28</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="27"/>
-    </row>
-    <row r="35" spans="1:7" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="28">
-        <v>29</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="27"/>
-    </row>
-    <row r="36" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="27"/>
-    </row>
-    <row r="37" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="28">
-        <v>30</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="33"/>
-      <c r="G37" s="27"/>
-    </row>
-    <row r="38" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="28">
-        <v>31</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F39" s="33"/>
-      <c r="G39" s="27"/>
-    </row>
-    <row r="40" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="32">
-        <v>32</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="26"/>
-      <c r="G41" s="27"/>
-    </row>
-    <row r="42" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="32">
-        <v>33</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="26"/>
-      <c r="G42" s="27"/>
-    </row>
-    <row r="43" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="32">
-        <v>34</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="26"/>
-      <c r="G43" s="27"/>
-    </row>
-    <row r="44" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="44" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="119.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>